<commit_message>
Fix 5.1Ohm PN of the 10K resistors
</commit_message>
<xml_diff>
--- a/PCB/v1.3/BOM_1_3.xlsx
+++ b/PCB/v1.3/BOM_1_3.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ultimate-nag52" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ultimate-nag52" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">R3, R5, R6, R7, R8, R9, R10, R11, R18, R19, R20, R21, R23, R28, R29, R30, R34, R35, R36, R37, R38, R43</t>
   </si>
   <si>
-    <t xml:space="preserve">0603WAF510KT5E</t>
+    <t xml:space="preserve">0603WAF1002T5E</t>
   </si>
   <si>
     <t xml:space="preserve">10K</t>
@@ -412,6 +412,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -471,12 +472,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -492,6 +497,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -499,809 +610,809 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C10" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topRight" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="90.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="90.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="0" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="B24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="B26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="B30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="0" t="s">
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="B33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="0" t="s">
+      <c r="B35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="0" t="s">
+      <c r="B36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="0" t="s">
+      <c r="B40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="0" t="s">
+      <c r="B41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="0" t="s">
+      <c r="B42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C43" s="0" t="s">
+      <c r="B43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C44" s="0" t="s">
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="B47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>